<commit_message>
new sheet, deleted arrow
</commit_message>
<xml_diff>
--- a/src/main/resources/tariffs2.1.xlsx
+++ b/src/main/resources/tariffs2.1.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="20835" windowHeight="9765"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="20835" windowHeight="9765" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="тарифы" sheetId="1" r:id="rId1"/>
+    <sheet name="пользователи" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>название</t>
   </si>
@@ -57,9 +56,6 @@
     <t>возможность подключиения онлайн-кинотеатра WINK вместо приставки</t>
   </si>
   <si>
-    <t>50ГБ, 2000 минут по РФ, 500 SMS\n Безлимитные соцсети и мессенджеры</t>
-  </si>
-  <si>
     <t>100 руб./мес. (аренда)\n 3990 руб.(покупка)</t>
   </si>
   <si>
@@ -103,16 +99,42 @@
   </si>
   <si>
     <t>100 руб./мес. (аренда) \n 10 руб./мес. (аренда Б/У)\n 175 руб./мес. (рассрочка на 24 месяца)\n 3500 руб.(покупка)</t>
+  </si>
+  <si>
+    <t>50ГБ, 1200 минут по РФ, 500 SMS\n Безлимитные соцсети и мессенджеры</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>имя</t>
+  </si>
+  <si>
+    <t>Интернет + ТВ + Мобильная связь</t>
+  </si>
+  <si>
+    <t>Интернет</t>
+  </si>
+  <si>
+    <t>Интернет + ТВ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -139,13 +161,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -449,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,16 +537,16 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
       </c>
       <c r="I2">
         <v>700</v>
@@ -530,7 +560,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -542,16 +572,16 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
       </c>
       <c r="I3">
         <v>900</v>
@@ -565,28 +595,28 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
         <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
       </c>
       <c r="I4">
         <v>350</v>
@@ -600,7 +630,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -612,16 +642,16 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
         <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
       </c>
       <c r="I5">
         <v>560</v>
@@ -635,7 +665,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -647,16 +677,16 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6">
         <v>400</v>
@@ -676,24 +706,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>